<commit_message>
Creación del proyecto base. Cambios menores en el análisis. Adaptación de los riesgos para incluirlos en el proyecto.
</commit_message>
<xml_diff>
--- a/Análisis de riesgos.xlsx
+++ b/Análisis de riesgos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\Universidad\21-22\TFG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\Universidad\21-22\TFG\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA06120-7965-43CD-AE44-FE03486B9499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE75B8-ED65-454A-87CC-580801129549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F3DEDD03-9D89-43D4-96B0-92ADD609C2DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{F3DEDD03-9D89-43D4-96B0-92ADD609C2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Activos" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Análisis de riesgos" sheetId="4" r:id="rId4"/>
     <sheet name="Hoja2" sheetId="5" r:id="rId5"/>
     <sheet name="Hoja3" sheetId="6" r:id="rId6"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="265">
   <si>
     <t>Código</t>
   </si>
@@ -312,9 +313,6 @@
   </si>
   <si>
     <t>Amenaza</t>
-  </si>
-  <si>
-    <t>Fecha de detección</t>
   </si>
   <si>
     <t>Riesgos</t>
@@ -820,6 +818,30 @@
   </si>
   <si>
     <t>Producto dista de lo esperado</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Respuesta a los Riesgos</t>
+  </si>
+  <si>
+    <t>Asumir</t>
+  </si>
+  <si>
+    <t>Las enfermedades son algo imprevisibles, el desarrollador está vacunado contra la gripe y el COVID-19, y dispone de mediacamentos para tratar los síntomas de las enfermedades menores</t>
+  </si>
+  <si>
+    <t>Prevención</t>
+  </si>
+  <si>
+    <t>Los datos se subirán a GitHub de forma diaria y se cuenta con equipos auxiliares donde se podría continuar con el trabajo.</t>
+  </si>
+  <si>
+    <t>Se fijarán reuniones semanales para bloquear horarios y asegurar un seguimiento del proyecto por parte de los tutores.</t>
+  </si>
+  <si>
+    <t>El desarrollador facilitará su correo electrónico personal a los tutores para poder comunicarse en caso de caída del servidor de correo de la universidad. Se utilizará otra herramienta de comunicación por videollamada como puede ser Discord o Zoom.</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1016,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1287,11 +1309,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1433,6 +1464,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1443,6 +1475,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1466,319 +1501,26 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2187,11 +1929,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2297,10 +2039,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2308,10 +2050,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -2319,10 +2061,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2469,11 +2211,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2578,10 +2320,10 @@
         <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2589,7 +2331,7 @@
         <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -2598,7 +2340,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -2607,7 +2349,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -2616,10 +2358,10 @@
         <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2627,10 +2369,10 @@
         <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2638,10 +2380,10 @@
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2649,10 +2391,10 @@
         <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2660,7 +2402,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -2669,7 +2411,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -2678,7 +2420,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C22" s="1"/>
     </row>
@@ -2687,7 +2429,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -2696,7 +2438,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" s="1"/>
     </row>
@@ -2705,7 +2447,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -2714,7 +2456,7 @@
         <v>74</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -2752,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56749D7C-F73E-41FB-8624-76538F1817E6}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" activeCellId="1" sqref="A33:XFD33 A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2763,21 +2505,21 @@
     <col min="3" max="3" width="66.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" style="68" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" style="70" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="A1" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="69"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2790,27 +2532,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>91</v>
-      </c>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>30</v>
@@ -2818,62 +2558,59 @@
       <c r="E3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>42</v>
@@ -2881,335 +2618,319 @@
       <c r="E6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" s="10"/>
+      <c r="F6" s="67" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>148</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>153</v>
-      </c>
       <c r="D10" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>159</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B17" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="D17" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="C18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>176</v>
-      </c>
       <c r="D19" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="C20" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="67" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="C21" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>30</v>
@@ -3217,352 +2938,333 @@
       <c r="E22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="67" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="67" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="C24" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F24" s="67" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F25" s="67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F26" s="67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F30" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>211</v>
-      </c>
       <c r="D31" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F31" s="67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="D33" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="B34" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="E35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="B36" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="D36" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="67" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="10"/>
       <c r="E37" s="11"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="67"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
       <c r="E38" s="11"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F38" s="67"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
       <c r="E39" s="11"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="67"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="10"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3615,15 +3317,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55" t="s">
-        <v>236</v>
-      </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
@@ -3633,122 +3335,122 @@
         <v>1</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D2" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>237</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="65">
+        <v>226</v>
+      </c>
+      <c r="E3" s="53">
         <f>VLOOKUP(C3,$M$6:$R$11,MATCH(D3,$M$6:$R$6,0),FALSE)</f>
         <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E4" s="65">
+        <v>227</v>
+      </c>
+      <c r="E4" s="53">
         <f t="shared" ref="E4:E33" si="0">VLOOKUP(C4,$M$6:$R$11,MATCH(D4,$M$6:$R$6,0),FALSE)</f>
         <v>0.17</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="65">
+        <v>225</v>
+      </c>
+      <c r="E5" s="53">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="65">
+        <v>225</v>
+      </c>
+      <c r="E6" s="53">
         <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="M6" s="51"/>
       <c r="N6" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O6" s="51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P6" s="51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q6" s="51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="R6" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E7" s="65">
+        <v>227</v>
+      </c>
+      <c r="E7" s="53">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
       <c r="M7" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N7" s="52">
         <v>0.68</v>
@@ -3768,23 +3470,23 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E8" s="65">
+        <v>227</v>
+      </c>
+      <c r="E8" s="53">
         <f t="shared" si="0"/>
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N8" s="52">
         <v>0.55249999999999999</v>
@@ -3804,23 +3506,23 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E9" s="65">
+        <v>225</v>
+      </c>
+      <c r="E9" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="M9" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N9" s="52">
         <v>0.34</v>
@@ -3840,23 +3542,23 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E10" s="65">
+        <v>226</v>
+      </c>
+      <c r="E10" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="M10" s="51" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N10" s="52">
         <v>0.17</v>
@@ -3876,23 +3578,23 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E11" s="65">
+        <v>227</v>
+      </c>
+      <c r="E11" s="53">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
       <c r="M11" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N11" s="52">
         <v>4.2500000000000003E-2</v>
@@ -3912,450 +3614,450 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="E12" s="65">
+        <v>224</v>
+      </c>
+      <c r="E12" s="53">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E13" s="65">
+        <v>226</v>
+      </c>
+      <c r="E13" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="65">
+        <v>225</v>
+      </c>
+      <c r="E14" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E15" s="65">
+        <v>227</v>
+      </c>
+      <c r="E15" s="53">
         <f t="shared" si="0"/>
         <v>0.55249999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E16" s="65">
+        <v>226</v>
+      </c>
+      <c r="E16" s="53">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="65">
+        <v>226</v>
+      </c>
+      <c r="E17" s="53">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E18" s="65">
+        <v>226</v>
+      </c>
+      <c r="E18" s="53">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E19" s="65">
+        <v>226</v>
+      </c>
+      <c r="E19" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" s="65">
+        <v>226</v>
+      </c>
+      <c r="E20" s="53">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E21" s="65">
+        <v>226</v>
+      </c>
+      <c r="E21" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E22" s="65">
+        <v>225</v>
+      </c>
+      <c r="E22" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E23" s="65">
+        <v>226</v>
+      </c>
+      <c r="E23" s="53">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E24" s="65">
+        <v>225</v>
+      </c>
+      <c r="E24" s="53">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E25" s="65">
+        <v>227</v>
+      </c>
+      <c r="E25" s="53">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E26" s="65">
+        <v>227</v>
+      </c>
+      <c r="E26" s="53">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E27" s="65">
+        <v>226</v>
+      </c>
+      <c r="E27" s="53">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" s="65">
+        <v>225</v>
+      </c>
+      <c r="E28" s="53">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E29" s="65">
+        <v>225</v>
+      </c>
+      <c r="E29" s="53">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="65">
+        <v>225</v>
+      </c>
+      <c r="E30" s="53">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E31" s="65">
+        <v>225</v>
+      </c>
+      <c r="E31" s="53">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E32" s="65">
+        <v>226</v>
+      </c>
+      <c r="E32" s="53">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E33" s="65">
+        <v>225</v>
+      </c>
+      <c r="E33" s="53">
         <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="E34" s="65">
+        <v>225</v>
+      </c>
+      <c r="E34" s="53">
         <f t="shared" ref="E34:E36" si="1">VLOOKUP(C34,$M$6:$R$11,MATCH(D34,$M$6:$R$6,0),FALSE)</f>
         <v>0.12</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E35" s="65">
+        <v>226</v>
+      </c>
+      <c r="E35" s="53">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E36" s="65">
+        <v>227</v>
+      </c>
+      <c r="E36" s="53">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
@@ -4367,7 +4069,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3:C36">
-    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="Muy Alta">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Muy Alta">
       <formula>NOT(ISERROR(SEARCH("Muy Alta",C3)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -4382,35 +4084,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C36">
-    <cfRule type="beginsWith" dxfId="18" priority="14" operator="beginsWith" text="Alta">
+    <cfRule type="beginsWith" dxfId="8" priority="14" operator="beginsWith" text="Alta">
       <formula>LEFT(C3,LEN("Alta"))="Alta"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C36">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="Insignificante">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Insignificante">
       <formula>NOT(ISERROR(SEARCH("Insignificante",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D36">
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Insignificante">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Insignificante">
       <formula>NOT(ISERROR(SEARCH("Insignificante",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Bajo">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Bajo">
       <formula>NOT(ISERROR(SEARCH("Bajo",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Medio">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Medio">
       <formula>NOT(ISERROR(SEARCH("Medio",D3)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="9" operator="beginsWith" text="Alto">
+    <cfRule type="beginsWith" dxfId="1" priority="9" operator="beginsWith" text="Alto">
       <formula>LEFT(D3,LEN("Alto"))="Alto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Muy alto">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="Muy alto">
       <formula>NOT(ISERROR(SEARCH("Muy alto",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4441,13 +4143,304 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381A10C6-6F24-4DF8-BCBF-B83CE5EBC6B5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="69"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="70"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="70"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="70"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="70"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="70"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="70"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="70"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="70"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="G12" s="70"/>
+      <c r="H12" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28A8FD2A-4E26-45AE-967A-653D73BBFFEF}">
+          <x14:formula1>
+            <xm:f>Activos!$B$3:$B$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F27B1C3-229A-46F3-B953-B089F3EC2F99}">
+          <x14:formula1>
+            <xm:f>Amenazas!$B$3:$B$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F11 F12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E28479A0-72BB-4E59-A8C7-E351A5084607}">
+          <x14:formula1>
+            <xm:f>Activos!$B$3:$B$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5:E11 E12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4481,36 +4474,36 @@
       <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
-        <v>229</v>
+      <c r="A2" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="64"/>
       <c r="M2" s="12"/>
-      <c r="N2" s="56" t="s">
-        <v>229</v>
+      <c r="N2" s="58" t="s">
+        <v>228</v>
       </c>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="13">
         <v>0.04</v>
@@ -4543,17 +4536,17 @@
         <v>0.04</v>
       </c>
       <c r="M3" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="N3" s="56"/>
+        <v>229</v>
+      </c>
+      <c r="N3" s="58"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="15">
         <v>3.2500000000000001E-2</v>
@@ -4586,17 +4579,17 @@
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="M4" s="39" t="s">
-        <v>231</v>
-      </c>
-      <c r="N4" s="56"/>
+        <v>230</v>
+      </c>
+      <c r="N4" s="58"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5" s="15">
         <v>0.02</v>
@@ -4629,17 +4622,17 @@
         <v>0.02</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="N5" s="56"/>
+        <v>231</v>
+      </c>
+      <c r="N5" s="58"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="15">
         <v>0.01</v>
@@ -4672,17 +4665,17 @@
         <v>0.01</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="N6" s="56"/>
+        <v>232</v>
+      </c>
+      <c r="N6" s="58"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="18">
         <v>2.5000000000000001E-3</v>
@@ -4715,9 +4708,9 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>234</v>
-      </c>
-      <c r="N7" s="56"/>
+        <v>233</v>
+      </c>
+      <c r="N7" s="58"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -4726,34 +4719,34 @@
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="E8" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="F8" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="G8" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="G8" s="42" t="s">
-        <v>228</v>
-      </c>
       <c r="H8" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I8" s="41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K8" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L8" s="41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
@@ -4803,20 +4796,20 @@
     <row r="10" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63" t="s">
-        <v>223</v>
-      </c>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -5331,4 +5324,285 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A0784C-EE73-4B27-8C96-29BBB7324E53}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75030BAA-220D-4745-BE22-5EF0F279B616}">
+          <x14:formula1>
+            <xm:f>Activos!$B$3:$B$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5:E12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5C44CE32-89B4-462F-A6D1-6CC4DBDE44D9}">
+          <x14:formula1>
+            <xm:f>Amenazas!$B$3:$B$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95C0BED5-0F2B-4C8B-B7E5-0A7CEAAB2D9D}">
+          <x14:formula1>
+            <xm:f>Activos!$B$3:$B$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Inserción de la funcionalidad de registro con validación por correo.
</commit_message>
<xml_diff>
--- a/Análisis de riesgos.xlsx
+++ b/Análisis de riesgos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\Universidad\21-22\TFG\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE75B8-ED65-454A-87CC-580801129549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6271B046-D0A2-4F84-9745-7550912BBB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{F3DEDD03-9D89-43D4-96B0-92ADD609C2DE}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="272">
   <si>
     <t>Código</t>
   </si>
@@ -842,6 +842,27 @@
   </si>
   <si>
     <t>El desarrollador facilitará su correo electrónico personal a los tutores para poder comunicarse en caso de caída del servidor de correo de la universidad. Se utilizará otra herramienta de comunicación por videollamada como puede ser Discord o Zoom.</t>
+  </si>
+  <si>
+    <t>Se realizará un análisis para asegurar que las tencnologías que se van a emplear sean compatibles entre sí a la hora de seleccionarlas. Para ello, se intentará buscar ejemplos de proyectos o tutoriales en los que se demuestre su compatibilidad.</t>
+  </si>
+  <si>
+    <t>Se intentará realizar la planificación lo más realista posible.</t>
+  </si>
+  <si>
+    <t>Plan de contingencia</t>
+  </si>
+  <si>
+    <t>En caso de que las APIs no sean compatibles, se desarrollará un chat simple utilizando la aplicación REST y almacenando los mensajes en su base de datos.</t>
+  </si>
+  <si>
+    <t>Dado que esto es un prototipo, la usabilidad no será una prioridad directa.</t>
+  </si>
+  <si>
+    <t>Se intentará hacer participe al cliente del proyecto, inlcuyéndolo en el análisis y en el diseño y pidiendole que los valide.</t>
+  </si>
+  <si>
+    <t>Se determinará cuales son los módulos prioritarios en la aplicación y cuales podrían ser prescindibles en caso de no poder desarrollar todos.</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1037,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1318,11 +1339,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1465,6 +1528,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1501,20 +1579,17 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1929,11 +2004,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2211,11 +2286,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2505,21 +2580,21 @@
     <col min="3" max="3" width="66.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" style="68" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" style="58" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2537,10 +2612,10 @@
       <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="69"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -2558,7 +2633,7 @@
       <c r="E3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="55" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2578,7 +2653,7 @@
       <c r="E4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="55" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2598,7 +2673,7 @@
       <c r="E5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="55" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2618,7 +2693,7 @@
       <c r="E6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="55" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2638,7 +2713,7 @@
       <c r="E7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="55" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2658,7 +2733,7 @@
       <c r="E8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="67" t="s">
+      <c r="F8" s="55" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2678,7 +2753,7 @@
       <c r="E9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="55" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2698,7 +2773,7 @@
       <c r="E10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="67" t="s">
+      <c r="F10" s="55" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2718,7 +2793,7 @@
       <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="67" t="s">
+      <c r="F11" s="55" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2738,7 +2813,7 @@
       <c r="E12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2758,7 +2833,7 @@
       <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="55" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2778,7 +2853,7 @@
       <c r="E14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="55" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2798,7 +2873,7 @@
       <c r="E15" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="67" t="s">
+      <c r="F15" s="55" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2818,7 +2893,7 @@
       <c r="E16" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="55" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2838,7 +2913,7 @@
       <c r="E17" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="55" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2858,7 +2933,7 @@
       <c r="E18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="67" t="s">
+      <c r="F18" s="55" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2878,7 +2953,7 @@
       <c r="E19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="67" t="s">
+      <c r="F19" s="55" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2898,7 +2973,7 @@
       <c r="E20" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="67" t="s">
+      <c r="F20" s="55" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2918,7 +2993,7 @@
       <c r="E21" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="67" t="s">
+      <c r="F21" s="55" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2938,7 +3013,7 @@
       <c r="E22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="67" t="s">
+      <c r="F22" s="55" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2958,7 +3033,7 @@
       <c r="E23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="67" t="s">
+      <c r="F23" s="55" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2978,7 +3053,7 @@
       <c r="E24" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="55" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2998,7 +3073,7 @@
       <c r="E25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="67" t="s">
+      <c r="F25" s="55" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3018,7 +3093,7 @@
       <c r="E26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="67" t="s">
+      <c r="F26" s="55" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3038,7 +3113,7 @@
       <c r="E27" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="67" t="s">
+      <c r="F27" s="55" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3058,7 +3133,7 @@
       <c r="E28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="67" t="s">
+      <c r="F28" s="55" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3078,7 +3153,7 @@
       <c r="E29" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="67" t="s">
+      <c r="F29" s="55" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3098,7 +3173,7 @@
       <c r="E30" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F30" s="67" t="s">
+      <c r="F30" s="55" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3118,7 +3193,7 @@
       <c r="E31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="67" t="s">
+      <c r="F31" s="55" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3138,7 +3213,7 @@
       <c r="E32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="67" t="s">
+      <c r="F32" s="55" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3158,7 +3233,7 @@
       <c r="E33" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="67" t="s">
+      <c r="F33" s="55" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3178,7 +3253,7 @@
       <c r="E34" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="67" t="s">
+      <c r="F34" s="55" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3198,7 +3273,7 @@
       <c r="E35" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="67" t="s">
+      <c r="F35" s="55" t="s">
         <v>247</v>
       </c>
     </row>
@@ -3218,7 +3293,7 @@
       <c r="E36" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="67" t="s">
+      <c r="F36" s="55" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3230,7 +3305,7 @@
       <c r="C37" s="11"/>
       <c r="D37" s="10"/>
       <c r="E37" s="11"/>
-      <c r="F37" s="67"/>
+      <c r="F37" s="55"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
@@ -3240,7 +3315,7 @@
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
       <c r="E38" s="11"/>
-      <c r="F38" s="67"/>
+      <c r="F38" s="55"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
@@ -3250,7 +3325,7 @@
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
       <c r="E39" s="11"/>
-      <c r="F39" s="67"/>
+      <c r="F39" s="55"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
@@ -3260,7 +3335,7 @@
       <c r="C40" s="11"/>
       <c r="D40" s="10"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="67"/>
+      <c r="F40" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3317,15 +3392,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
@@ -4159,15 +4234,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="57"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4186,10 +4261,10 @@
       <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="69"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4208,10 +4283,10 @@
       <c r="E3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="70"/>
+      <c r="G3" s="58"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4230,10 +4305,10 @@
       <c r="E4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="70"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4252,10 +4327,10 @@
       <c r="E5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="G5" s="70"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4274,10 +4349,10 @@
       <c r="E6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="70"/>
+      <c r="G6" s="58"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4296,10 +4371,10 @@
       <c r="E7" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="70"/>
+      <c r="G7" s="58"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4318,10 +4393,10 @@
       <c r="E8" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="67" t="s">
+      <c r="F8" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="70"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4340,10 +4415,10 @@
       <c r="E9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="70"/>
+      <c r="G9" s="58"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4362,10 +4437,10 @@
       <c r="E10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="67" t="s">
+      <c r="F10" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="70"/>
+      <c r="G10" s="58"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -4384,10 +4459,10 @@
       <c r="E11" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F11" s="67" t="s">
+      <c r="F11" s="55" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="70"/>
+      <c r="G11" s="58"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4406,10 +4481,10 @@
       <c r="E12" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="55" t="s">
         <v>217</v>
       </c>
-      <c r="G12" s="70"/>
+      <c r="G12" s="58"/>
       <c r="H12" s="6"/>
     </row>
   </sheetData>
@@ -4474,26 +4549,26 @@
       <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="62" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="12"/>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="63" t="s">
         <v>228</v>
       </c>
       <c r="O2" s="12"/>
@@ -4501,7 +4576,7 @@
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="39" t="s">
         <v>229</v>
       </c>
@@ -4538,13 +4613,13 @@
       <c r="M3" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="N3" s="58"/>
+      <c r="N3" s="63"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="39" t="s">
         <v>230</v>
       </c>
@@ -4581,13 +4656,13 @@
       <c r="M4" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="N4" s="58"/>
+      <c r="N4" s="63"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="39" t="s">
         <v>231</v>
       </c>
@@ -4624,13 +4699,13 @@
       <c r="M5" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="N5" s="58"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="39" t="s">
         <v>232</v>
       </c>
@@ -4667,13 +4742,13 @@
       <c r="M6" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="N6" s="58"/>
+      <c r="N6" s="63"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="57"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="39" t="s">
         <v>233</v>
       </c>
@@ -4710,7 +4785,7 @@
       <c r="M7" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="N7" s="58"/>
+      <c r="N7" s="63"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -4796,20 +4871,20 @@
     <row r="10" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65" t="s">
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70" t="s">
         <v>222</v>
       </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -5328,34 +5403,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A0784C-EE73-4B27-8C96-29BBB7324E53}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="71" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5367,14 +5438,8 @@
       <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>92</v>
       </c>
@@ -5387,14 +5452,8 @@
       <c r="D3" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>93</v>
       </c>
@@ -5407,14 +5466,8 @@
       <c r="D4" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>95</v>
       </c>
@@ -5427,14 +5480,8 @@
       <c r="D5" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="67" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>99</v>
       </c>
@@ -5447,14 +5494,8 @@
       <c r="D6" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="67" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>104</v>
       </c>
@@ -5462,19 +5503,13 @@
         <v>161</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>105</v>
       </c>
@@ -5482,19 +5517,13 @@
         <v>167</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>116</v>
       </c>
@@ -5502,19 +5531,13 @@
         <v>190</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>138</v>
+        <v>261</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>117</v>
       </c>
@@ -5522,19 +5545,13 @@
         <v>191</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>138</v>
+        <v>267</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>122</v>
       </c>
@@ -5542,19 +5559,13 @@
         <v>207</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="67" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>123</v>
       </c>
@@ -5562,47 +5573,17 @@
         <v>242</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="67" t="s">
-        <v>217</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75030BAA-220D-4745-BE22-5EF0F279B616}">
-          <x14:formula1>
-            <xm:f>Activos!$B$3:$B$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>E5:E12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5C44CE32-89B4-462F-A6D1-6CC4DBDE44D9}">
-          <x14:formula1>
-            <xm:f>Amenazas!$B$3:$B$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95C0BED5-0F2B-4C8B-B7E5-0A7CEAAB2D9D}">
-          <x14:formula1>
-            <xm:f>Activos!$B$3:$B$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se continúa elaborando la memoria. Mejoras menores en la aplicación y solución de pequeños errores.
</commit_message>
<xml_diff>
--- a/Análisis de riesgos.xlsx
+++ b/Análisis de riesgos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\Universidad\21-22\TFG\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6271B046-D0A2-4F84-9745-7550912BBB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE338B8-56E1-41E6-B9E7-9DCAC8696D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{F3DEDD03-9D89-43D4-96B0-92ADD609C2DE}"/>
   </bookViews>
@@ -832,9 +832,6 @@
     <t>Las enfermedades son algo imprevisibles, el desarrollador está vacunado contra la gripe y el COVID-19, y dispone de mediacamentos para tratar los síntomas de las enfermedades menores</t>
   </si>
   <si>
-    <t>Prevención</t>
-  </si>
-  <si>
     <t>Los datos se subirán a GitHub de forma diaria y se cuenta con equipos auxiliares donde se podría continuar con el trabajo.</t>
   </si>
   <si>
@@ -863,6 +860,9 @@
   </si>
   <si>
     <t>Se determinará cuales son los módulos prioritarios en la aplicación y cuales podrían ser prescindibles en caso de no poder desarrollar todos.</t>
+  </si>
+  <si>
+    <t>Mitigación</t>
   </si>
 </sst>
 </file>
@@ -1543,6 +1543,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,9 +1589,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2004,11 +2004,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2286,11 +2286,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2586,14 +2586,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3392,15 +3392,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
@@ -4234,14 +4234,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="57"/>
       <c r="H1" s="6"/>
     </row>
@@ -4549,26 +4549,26 @@
       <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="12"/>
-      <c r="N2" s="63" t="s">
+      <c r="N2" s="64" t="s">
         <v>228</v>
       </c>
       <c r="O2" s="12"/>
@@ -4576,7 +4576,7 @@
       <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="39" t="s">
         <v>229</v>
       </c>
@@ -4613,13 +4613,13 @@
       <c r="M3" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="N3" s="63"/>
+      <c r="N3" s="64"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="39" t="s">
         <v>230</v>
       </c>
@@ -4656,13 +4656,13 @@
       <c r="M4" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="N4" s="63"/>
+      <c r="N4" s="64"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="39" t="s">
         <v>231</v>
       </c>
@@ -4699,13 +4699,13 @@
       <c r="M5" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="N5" s="63"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="39" t="s">
         <v>232</v>
       </c>
@@ -4742,13 +4742,13 @@
       <c r="M6" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="N6" s="63"/>
+      <c r="N6" s="64"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="39" t="s">
         <v>233</v>
       </c>
@@ -4785,7 +4785,7 @@
       <c r="M7" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="N7" s="63"/>
+      <c r="N7" s="64"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -4871,20 +4871,20 @@
     <row r="10" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -5406,7 +5406,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5418,15 +5418,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="72" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5461,10 +5461,10 @@
         <v>136</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5475,10 +5475,10 @@
         <v>141</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5489,10 +5489,10 @@
         <v>151</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5503,10 +5503,10 @@
         <v>161</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5517,10 +5517,10 @@
         <v>167</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5531,10 +5531,10 @@
         <v>190</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -5545,10 +5545,10 @@
         <v>191</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -5559,10 +5559,10 @@
         <v>207</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -5576,7 +5576,7 @@
         <v>259</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>